<commit_message>
Continuation du registre de risques
</commit_message>
<xml_diff>
--- a/Remises/Remise 2/GestionRisques.xlsx
+++ b/Remises/Remise 2/GestionRisques.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
   <si>
     <t>Type de risque</t>
   </si>
@@ -138,6 +138,78 @@
   </si>
   <si>
     <t>X. Kedzierski</t>
+  </si>
+  <si>
+    <t>Décodage erroné du code Manchester</t>
+  </si>
+  <si>
+    <t>Impossibilité de recevoir la bonne description de l'île mystère</t>
+  </si>
+  <si>
+    <t>Possibilité de recevoir et décoder plusieurs fois le code avant de l'envoyer au serveur et donc d'éliminer les mauvais décodages</t>
+  </si>
+  <si>
+    <t>Échec d'ouverture et/ou lancement du programme à l'ouverture du mini-pc</t>
+  </si>
+  <si>
+    <t>Impossibilité de commencer la tâche</t>
+  </si>
+  <si>
+    <t>Possibilité de désactiver les mises à jour sur le système d'exploitation</t>
+  </si>
+  <si>
+    <t>Échec de la connection entre la station de base et le robot</t>
+  </si>
+  <si>
+    <t>Impossibilité d'afficher les données transmisses par le robot</t>
+  </si>
+  <si>
+    <t>Possibilité d'établir une routine de tentatives de connections suite à un échec comme pour le serveur des îles</t>
+  </si>
+  <si>
+    <t>Perte des points liés à l'affichage des données</t>
+  </si>
+  <si>
+    <t>Trésor échappé par le robot</t>
+  </si>
+  <si>
+    <t>Perte d'un trésor et nécessiter de recharger le condensateur en plus de trouver un autre trésor</t>
+  </si>
+  <si>
+    <t>Perte de temps lors de l'essai et possibilité de manquer de temps</t>
+  </si>
+  <si>
+    <t>Tester le temps de décharge du condensateur lorsque l'électroaimant est solicité. Possibilité de prendre un condensateur de capacité plus élevé</t>
+  </si>
+  <si>
+    <t>E. Bourque</t>
+  </si>
+  <si>
+    <t>Bris d'un équipement fourni pour le projet</t>
+  </si>
+  <si>
+    <t>Nécessité de trouver un équipement de remplacement</t>
+  </si>
+  <si>
+    <t>Performances réduites si le nouvel équipement est moins performant</t>
+  </si>
+  <si>
+    <t>20$/membre + nouvel équipement</t>
+  </si>
+  <si>
+    <t>Nécessité de lire les fiches techniques de chaque appareil pour tout les membres ainsi que de ranger correctement l'équipement</t>
+  </si>
+  <si>
+    <t>Perte d'un membre d'équipe (abandon, hospitalisation, etc)</t>
+  </si>
+  <si>
+    <t>Nécessité pour les autres membres de se partager la tâche du membre manquant</t>
+  </si>
+  <si>
+    <t>Systèmes moins performants ou moins testés par manque de temps des autres membres</t>
+  </si>
+  <si>
+    <t>Documenter son avancement pour chaque système conçu individuellement afin de faciliter la reprise du travail par un autre membre de l'équipe</t>
   </si>
 </sst>
 </file>
@@ -242,40 +314,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -583,316 +664,402 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.77734375" customWidth="1"/>
     <col min="3" max="3" width="21.109375" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" customWidth="1"/>
     <col min="5" max="5" width="23.88671875" customWidth="1"/>
     <col min="6" max="6" width="15.109375" customWidth="1"/>
     <col min="7" max="7" width="15.88671875" customWidth="1"/>
-    <col min="8" max="8" width="31.21875" customWidth="1"/>
+    <col min="8" max="8" width="34.21875" customWidth="1"/>
     <col min="9" max="9" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
     </row>
     <row r="4" spans="2:9" ht="58.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="7">
         <v>0.05</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="13"/>
+      <c r="H4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="2">
         <v>5</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="8">
         <v>0.3</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="8" t="s">
+      <c r="G5" s="12"/>
+      <c r="H5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="2">
         <v>2</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="8">
         <v>0.1</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="8" t="s">
+      <c r="G6" s="12"/>
+      <c r="H6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="8">
         <v>0.05</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="8" t="s">
+      <c r="G7" s="12"/>
+      <c r="H7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="2">
         <v>5</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="2">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="G9" s="12"/>
+      <c r="H9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="H10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="8">
         <v>0.1</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="5" t="s">
+      <c r="G11" s="12"/>
+      <c r="H11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="2">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="5">
-        <v>5</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="11">
+    <row r="13" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="2">
+        <v>3</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="8">
         <v>0.05</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="B10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="5">
-        <v>3</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="11">
+      <c r="G13" s="12"/>
+      <c r="H13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="2">
+        <v>4</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="8">
         <v>0.15</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="8"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="8"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="8"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="8"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="8"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="8"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="5"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="G16" s="12"/>
+      <c r="H16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="8"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="2"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="8"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="9"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
ajustement gantt et gestion risque
</commit_message>
<xml_diff>
--- a/Remises/Remise 2/GestionRisques.xlsx
+++ b/Remises/Remise 2/GestionRisques.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
   <si>
     <t>Type de risque</t>
   </si>
@@ -210,6 +210,30 @@
   </si>
   <si>
     <t>Documenter son avancement pour chaque système conçu individuellement afin de faciliter la reprise du travail par un autre membre de l'équipe</t>
+  </si>
+  <si>
+    <t>Non respect des délais de livraison des documents à produire pour les livrables</t>
+  </si>
+  <si>
+    <t>Nécessité par les autres membres de terminer le travail pour les autres ou devoir remettre un livrable incomplet</t>
+  </si>
+  <si>
+    <t>Perte de points liés aux sections manquantes ou moins raffinées du livrable</t>
+  </si>
+  <si>
+    <t>Vérification périodique de l'avancement des travaux par le chef d'équipe ainsi que mise en place d'un "deadline" pour la remise des travaux un jour ou deux avant la remise du livrable</t>
+  </si>
+  <si>
+    <t>Dépassement du budget du projet</t>
+  </si>
+  <si>
+    <t>Nécessité de retirer des pièces du robot pour arriver en dessous du 300$ imposé</t>
+  </si>
+  <si>
+    <t>Assigner à un membre de l'équipe la charge de conserver un relevé du coût des pièces placées sur le robot ainsi que les factures</t>
+  </si>
+  <si>
+    <t>Performances réduites si le nouvel équipement de remplacement est moins performant ou plus complexe à intégrer</t>
   </si>
 </sst>
 </file>
@@ -340,6 +364,15 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -348,15 +381,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -664,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -673,7 +697,7 @@
     <col min="1" max="1" width="4.33203125" customWidth="1"/>
     <col min="2" max="2" width="26.77734375" customWidth="1"/>
     <col min="3" max="3" width="21.109375" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
     <col min="5" max="5" width="23.88671875" customWidth="1"/>
     <col min="6" max="6" width="15.109375" customWidth="1"/>
     <col min="7" max="7" width="15.88671875" customWidth="1"/>
@@ -682,42 +706,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="2:9" ht="58.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+    </row>
+    <row r="4" spans="2:9" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
@@ -733,12 +757,12 @@
       <c r="F4" s="7">
         <v>0.05</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="10"/>
       <c r="H4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -757,7 +781,7 @@
       <c r="F5" s="8">
         <v>0.3</v>
       </c>
-      <c r="G5" s="12"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="5" t="s">
         <v>16</v>
       </c>
@@ -781,7 +805,7 @@
       <c r="F6" s="8">
         <v>0.1</v>
       </c>
-      <c r="G6" s="12"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="5" t="s">
         <v>20</v>
       </c>
@@ -805,7 +829,7 @@
       <c r="F7" s="8">
         <v>0.05</v>
       </c>
-      <c r="G7" s="12"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="5" t="s">
         <v>26</v>
       </c>
@@ -829,7 +853,7 @@
       <c r="F8" s="8">
         <v>0.05</v>
       </c>
-      <c r="G8" s="12"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="5" t="s">
         <v>29</v>
       </c>
@@ -853,7 +877,7 @@
       <c r="F9" s="8">
         <v>0.05</v>
       </c>
-      <c r="G9" s="12"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="5" t="s">
         <v>33</v>
       </c>
@@ -877,7 +901,7 @@
       <c r="F10" s="8">
         <v>0.15</v>
       </c>
-      <c r="G10" s="12"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="5" t="s">
         <v>37</v>
       </c>
@@ -901,7 +925,7 @@
       <c r="F11" s="8">
         <v>0.1</v>
       </c>
-      <c r="G11" s="12"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="5" t="s">
         <v>41</v>
       </c>
@@ -925,7 +949,7 @@
       <c r="F12" s="8">
         <v>0.05</v>
       </c>
-      <c r="G12" s="12"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="5" t="s">
         <v>44</v>
       </c>
@@ -933,7 +957,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>45</v>
       </c>
@@ -949,7 +973,7 @@
       <c r="F13" s="8">
         <v>0.05</v>
       </c>
-      <c r="G13" s="12"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="5" t="s">
         <v>47</v>
       </c>
@@ -957,7 +981,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>49</v>
       </c>
@@ -973,7 +997,7 @@
       <c r="F14" s="8">
         <v>0.15</v>
       </c>
-      <c r="G14" s="12"/>
+      <c r="G14" s="9"/>
       <c r="H14" s="5" t="s">
         <v>52</v>
       </c>
@@ -997,7 +1021,7 @@
       <c r="F15" s="8">
         <v>0.02</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="9" t="s">
         <v>57</v>
       </c>
       <c r="H15" s="5" t="s">
@@ -1023,7 +1047,7 @@
       <c r="F16" s="8">
         <v>0.02</v>
       </c>
-      <c r="G16" s="12"/>
+      <c r="G16" s="9"/>
       <c r="H16" s="5" t="s">
         <v>62</v>
       </c>
@@ -1031,25 +1055,53 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="5"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="5"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="2"/>
+    <row r="17" spans="2:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="B17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="2">
+        <v>5</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="6"/>
@@ -1057,7 +1109,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="14"/>
+      <c r="G19" s="11"/>
       <c r="H19" s="6"/>
       <c r="I19" s="3"/>
     </row>

</xml_diff>

<commit_message>
ajustements gestion de risques
</commit_message>
<xml_diff>
--- a/Remises/Remise 2/GestionRisques.xlsx
+++ b/Remises/Remise 2/GestionRisques.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="97">
   <si>
     <t>Type de risque</t>
   </si>
@@ -35,10 +35,6 @@
 d'occurrence</t>
   </si>
   <si>
-    <t>Coût estimé 
-du risque ($)</t>
-  </si>
-  <si>
     <t>Plan de réduction
 du risque</t>
   </si>
@@ -83,9 +79,6 @@
     <t>Malfonctions et/ou dommages aux systèmes</t>
   </si>
   <si>
-    <t>Identifier les bornes de branchement et les différents fils</t>
-  </si>
-  <si>
     <t>J. Brown</t>
   </si>
   <si>
@@ -234,6 +227,91 @@
   </si>
   <si>
     <t>Performances réduites si le nouvel équipement de remplacement est moins performant ou plus complexe à intégrer</t>
+  </si>
+  <si>
+    <t>Coût estimé 
+du risque</t>
+  </si>
+  <si>
+    <t>Mauvaise estimation du temps de travail nécessaire à un système</t>
+  </si>
+  <si>
+    <t>Nécessité de passer plus de temps sur le système correspondant</t>
+  </si>
+  <si>
+    <t>Perte de temps de travail sur d'autres systèmes</t>
+  </si>
+  <si>
+    <t>Évaluer hebdomadairement l'avancement du travail de chacun et attribution de ressources supplémentaires pour finir le travail</t>
+  </si>
+  <si>
+    <t>Perte des factures détaillants les achats</t>
+  </si>
+  <si>
+    <t>Possibilité de non-remboursement et difficulté de justification du coût du robot</t>
+  </si>
+  <si>
+    <t>Échec du critère sur le coût</t>
+  </si>
+  <si>
+    <t>Mauvaise communication entre les membres de l'équipe</t>
+  </si>
+  <si>
+    <t>Possibilité de faire du travail en double ou de faire une tâche non nécessaire</t>
+  </si>
+  <si>
+    <t>Perte de temps de travail</t>
+  </si>
+  <si>
+    <t>Possibilité de photocopier les factures</t>
+  </si>
+  <si>
+    <t>Réaliser un compte rendu de chaque réunion et de la tâche de chacun par un secrétaire</t>
+  </si>
+  <si>
+    <t>C. Magnan</t>
+  </si>
+  <si>
+    <t>Manque de motivation de l'équipe</t>
+  </si>
+  <si>
+    <t>Manque de volonté à travailler sur le projet</t>
+  </si>
+  <si>
+    <t>Perte de temps de travail et travail bâclé</t>
+  </si>
+  <si>
+    <t>Possibilité par chaque membre de discuter en réunion des avancements de sa charge de travail pour conserver l'intérêt des autres et chercher de l'aide en cas de besoin</t>
+  </si>
+  <si>
+    <t>Défectuosité d'une pièce lors de la réception ou de l'achat de celle-ci</t>
+  </si>
+  <si>
+    <t>Nécessité de racheter la pièce</t>
+  </si>
+  <si>
+    <t>Perte de temps de test et de conception</t>
+  </si>
+  <si>
+    <t>10-20$/membre</t>
+  </si>
+  <si>
+    <t>Éviter d'acheter des pièces avec des délais de livraison important</t>
+  </si>
+  <si>
+    <t>Identifier les bornes de branchement et les différents fils par un système de couleur</t>
+  </si>
+  <si>
+    <t>Échec de l'integration entre 2 systèmes</t>
+  </si>
+  <si>
+    <t>Nécessité de modifier ou de changer complètement de système</t>
+  </si>
+  <si>
+    <t>Perte de temps de travail et de performance si le nouveau système est moins bon</t>
+  </si>
+  <si>
+    <t>Vérifier les fiches techniques des produits pour vérifier leur compatibilité avec d'autres systèmes</t>
   </si>
 </sst>
 </file>
@@ -257,7 +335,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -334,11 +412,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -346,9 +437,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -382,8 +470,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -689,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I18"/>
+  <dimension ref="B2:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,402 +812,591 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="12" t="s">
+    </row>
+    <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+    </row>
+    <row r="4" spans="2:9" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-    </row>
-    <row r="4" spans="2:9" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>13</v>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="C5" s="2">
         <v>5</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="8">
-        <v>0.3</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="2" t="s">
+    </row>
+    <row r="6" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B6" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="2" t="s">
+    </row>
+    <row r="7" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="I7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="C8" s="2">
         <v>5</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="5" t="s">
+    </row>
+    <row r="9" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B9" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="C9" s="2">
         <v>5</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="C10" s="2">
         <v>3</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="I10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="5" t="s">
+    </row>
+    <row r="11" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="C11" s="2">
         <v>3</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B12" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="C12" s="2">
         <v>5</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B13" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="C13" s="2">
         <v>3</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <v>0.05</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="5" t="s">
+      <c r="G13" s="8"/>
+      <c r="H13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="C14" s="2">
         <v>4</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="I14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="5" t="s">
+    </row>
+    <row r="15" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="C15" s="2">
         <v>4</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="H15" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="G15" s="9" t="s">
+      <c r="I15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="C16" s="2">
         <v>2</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="I16" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="B17" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="F16" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="B17" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="C17" s="2">
         <v>5</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="I17" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="B18" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="G17" s="9"/>
-      <c r="H17" s="5" t="s">
+      <c r="C18" s="15">
+        <v>3</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="B18" s="6" t="s">
+      <c r="E18" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="16">
+        <v>0.05</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="3">
+      <c r="I18" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="8">
+        <v>2</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="8">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" s="19">
+        <v>0.02</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="8">
         <v>3</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="15">
+      <c r="D21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="19">
         <v>0.05</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="B22" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="8">
+        <v>2</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B23" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="8">
+        <v>2</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="19">
+        <v>0.02</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="8">
+        <v>5</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="G24" s="8"/>
+      <c r="H24" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="4"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="4"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="8"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B27" s="4"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B28" s="5"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="10"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I29" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>